<commit_message>
Common: Improved job stuff
</commit_message>
<xml_diff>
--- a/fixtures/translations.xlsx
+++ b/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECE4D49-5CE4-4305-9C44-3D4193CE75A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB16345E-8F7E-446A-BEDB-2AFB3FB4F245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="1710" windowWidth="36270" windowHeight="18390" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1890" yWindow="1710" windowWidth="36270" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3471" uniqueCount="1778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3471" uniqueCount="1779">
   <si>
     <t>cs</t>
   </si>
@@ -5375,6 +5375,9 @@
   </si>
   <si>
     <t>root.job.title</t>
+  </si>
+  <si>
+    <t>translation2</t>
   </si>
 </sst>
 </file>
@@ -5730,8 +5733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6120BD2C-6516-4E86-99D3-11A27B514E61}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5777,7 +5780,7 @@
         <v>1768</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -6232,7 +6235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
   <dimension ref="A1:C986"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A958" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -17098,7 +17101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17153922-55B5-46AD-9C90-5ED46DB8719C}">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
@@ -17966,7 +17969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56FAEBF3-753C-4AE9-A2FF-818B5E33C44A}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Common: Improved some stuff
</commit_message>
<xml_diff>
--- a/fixtures/translations.xlsx
+++ b/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369CB600-6817-4E86-97BA-BFEE8AE04811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CE72B5-B10B-47CB-B88D-DBCFF3183AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="1710" windowWidth="36270" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1890" yWindow="1710" windowWidth="36270" windowHeight="18390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3471" uniqueCount="1778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3474" uniqueCount="1780">
   <si>
     <t>cs</t>
   </si>
@@ -5375,6 +5375,12 @@
   </si>
   <si>
     <t>root.job.title</t>
+  </si>
+  <si>
+    <t>common.filter.Jobs.filter.title</t>
+  </si>
+  <si>
+    <t>Filtrovat úlohy</t>
   </si>
 </sst>
 </file>
@@ -5730,7 +5736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6120BD2C-6516-4E86-99D3-11A27B514E61}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -5862,10 +5868,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6029,8 +6035,20 @@
         <v>152</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1778</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1779</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Common: A lot of improvements, going back to the track
</commit_message>
<xml_diff>
--- a/fixtures/translations.xlsx
+++ b/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CE72B5-B10B-47CB-B88D-DBCFF3183AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEB26C9-96EF-4A12-8F5F-1151E34EF0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1890" yWindow="1710" windowWidth="36270" windowHeight="18390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3474" uniqueCount="1780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3501" uniqueCount="1796">
   <si>
     <t>cs</t>
   </si>
@@ -5381,6 +5381,54 @@
   </si>
   <si>
     <t>Filtrovat úlohy</t>
+  </si>
+  <si>
+    <t>common.job.status.NEW</t>
+  </si>
+  <si>
+    <t>common.job.status.DONE</t>
+  </si>
+  <si>
+    <t>common.job.status.RUNNING</t>
+  </si>
+  <si>
+    <t>Probíhá</t>
+  </si>
+  <si>
+    <t>common.job.status.FAILURE</t>
+  </si>
+  <si>
+    <t>Selhání</t>
+  </si>
+  <si>
+    <t>common.job.cleanup.button</t>
+  </si>
+  <si>
+    <t>Vyčistit úlohy</t>
+  </si>
+  <si>
+    <t>common.job.commit-all.button</t>
+  </si>
+  <si>
+    <t>Potvrdit úlohy</t>
+  </si>
+  <si>
+    <t>common.job.cleanup.success</t>
+  </si>
+  <si>
+    <t>Úlohy byly úspěšně  vyčištěny.</t>
+  </si>
+  <si>
+    <t>common.job.status.SUCCESS</t>
+  </si>
+  <si>
+    <t>Úspěch</t>
+  </si>
+  <si>
+    <t>Úlohy byly úspěšně  označeny jako dokončené.</t>
+  </si>
+  <si>
+    <t>common.job.commit-all.success</t>
   </si>
 </sst>
 </file>
@@ -5868,10 +5916,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6044,6 +6092,105 @@
       </c>
       <c r="C15" s="1" t="s">
         <v>1779</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1780</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1781</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1782</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1784</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1786</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1788</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1795</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Job stuff is quite nice now
</commit_message>
<xml_diff>
--- a/fixtures/translations.xlsx
+++ b/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEB26C9-96EF-4A12-8F5F-1151E34EF0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000D2A9D-5EA9-4CA3-8798-008EBD1F4A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="1710" windowWidth="36270" windowHeight="18390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1890" yWindow="1710" windowWidth="36270" windowHeight="18390" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3501" uniqueCount="1796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3531" uniqueCount="1813">
   <si>
     <t>cs</t>
   </si>
@@ -5429,6 +5429,57 @@
   </si>
   <si>
     <t>common.job.commit-all.success</t>
+  </si>
+  <si>
+    <t>common.job.status.REVIEW</t>
+  </si>
+  <si>
+    <t>Ke kontrole</t>
+  </si>
+  <si>
+    <t>common.job.filter.status.label</t>
+  </si>
+  <si>
+    <t>Stav úlohy</t>
+  </si>
+  <si>
+    <t>common.job.filter.common.filter.submit</t>
+  </si>
+  <si>
+    <t>root.import.upload.error</t>
+  </si>
+  <si>
+    <t>Upload importního souboru se nezdařil.</t>
+  </si>
+  <si>
+    <t>common.job.status.RUNNING.tab</t>
+  </si>
+  <si>
+    <t>Běžící</t>
+  </si>
+  <si>
+    <t>common.job.status.FAILURE.tab</t>
+  </si>
+  <si>
+    <t>Selhané</t>
+  </si>
+  <si>
+    <t>common.job.status.SUCCESS.tab</t>
+  </si>
+  <si>
+    <t>Úspěšné</t>
+  </si>
+  <si>
+    <t>common.job.status.REVIEW.tab</t>
+  </si>
+  <si>
+    <t>common.job.status.DONE.tab</t>
+  </si>
+  <si>
+    <t>Dokončené</t>
+  </si>
+  <si>
+    <t>common.job.status.ALL.tab</t>
   </si>
 </sst>
 </file>
@@ -5916,10 +5967,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6191,6 +6242,39 @@
       </c>
       <c r="C24" s="1" t="s">
         <v>1794</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1796</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1798</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>902</v>
       </c>
     </row>
   </sheetData>
@@ -17261,10 +17345,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17153922-55B5-46AD-9C90-5ED46DB8719C}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18119,6 +18203,83 @@
       </c>
       <c r="C77" s="1" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>1805</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>1807</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>1809</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>1810</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>1812</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>1202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Some cool refactoring
</commit_message>
<xml_diff>
--- a/fixtures/translations.xlsx
+++ b/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB156E26-09FD-4FBF-97F1-6771353FDB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E2D212-5C53-4FDD-B773-57BC5889053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1890" yWindow="1710" windowWidth="36270" windowHeight="18390" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3534" uniqueCount="1814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3537" uniqueCount="1815">
   <si>
     <t>cs</t>
   </si>
@@ -5483,6 +5483,9 @@
   </si>
   <si>
     <t>root.file.title</t>
+  </si>
+  <si>
+    <t>root.user.title</t>
   </si>
 </sst>
 </file>
@@ -17348,10 +17351,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17153922-55B5-46AD-9C90-5ED46DB8719C}">
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18294,6 +18297,17 @@
       </c>
       <c r="C85" s="1" t="s">
         <v>124</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Whoo, file download works!
</commit_message>
<xml_diff>
--- a/fixtures/translations.xlsx
+++ b/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E2D212-5C53-4FDD-B773-57BC5889053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA5A8FD-0A21-4CE8-8C02-50B2121F603E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1890" yWindow="1710" windowWidth="36270" windowHeight="18390" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3537" uniqueCount="1815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3540" uniqueCount="1817">
   <si>
     <t>cs</t>
   </si>
@@ -5486,6 +5486,12 @@
   </si>
   <si>
     <t>root.user.title</t>
+  </si>
+  <si>
+    <t>shared.file.download</t>
+  </si>
+  <si>
+    <t>Stáhnout soubor</t>
   </si>
 </sst>
 </file>
@@ -17351,7 +17357,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17153922-55B5-46AD-9C90-5ED46DB8719C}">
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
       <selection activeCell="B82" sqref="B82"/>
@@ -18308,6 +18314,17 @@
       </c>
       <c r="C86" s="1" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>1816</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Just some texts on public
</commit_message>
<xml_diff>
--- a/fixtures/translations.xlsx
+++ b/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BCFE2F-7FF1-4CA0-A2CE-3217C7FD68CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F92AB72-0A89-4D10-9E17-091D1F5C11DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="1710" windowWidth="36270" windowHeight="18390" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2070" yWindow="2835" windowWidth="27960" windowHeight="18390" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3546" uniqueCount="1820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3597" uniqueCount="1850">
   <si>
     <t>cs</t>
   </si>
@@ -5392,9 +5392,6 @@
     <t>common.job.status.RUNNING</t>
   </si>
   <si>
-    <t>Probíhá</t>
-  </si>
-  <si>
     <t>common.job.status.FAILURE</t>
   </si>
   <si>
@@ -5501,6 +5498,120 @@
   </si>
   <si>
     <t>public.index.title</t>
+  </si>
+  <si>
+    <t>public.sing-in.card.title</t>
+  </si>
+  <si>
+    <t>Přihlášení</t>
+  </si>
+  <si>
+    <t>public.sign-in.github.button</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>public.home.menu</t>
+  </si>
+  <si>
+    <t>public.about.menu</t>
+  </si>
+  <si>
+    <t>O aplikaci</t>
+  </si>
+  <si>
+    <t>public.tos.menu</t>
+  </si>
+  <si>
+    <t>Podmínky použití</t>
+  </si>
+  <si>
+    <t>Probíhá (úspěch {{data.success}} / selhané {{data.failure}} / přeskočené {{data.skip}} z {{data.total}})</t>
+  </si>
+  <si>
+    <t>public.tos.title</t>
+  </si>
+  <si>
+    <t>public.about.title</t>
+  </si>
+  <si>
+    <t>public.intro.item.1.title</t>
+  </si>
+  <si>
+    <t>public.intro.item.1.content</t>
+  </si>
+  <si>
+    <t>Tato aplikace je určena všem vaperům, kteří touží po co nejlepším požitku z vapování. Nabízí řadu nástrojů, jejichž cílem je napomoci trasovat co nejvíce faktorů k odladění perfektního buildu.</t>
+  </si>
+  <si>
+    <t>public.intro.login.title</t>
+  </si>
+  <si>
+    <t>Možnosti přihlášení</t>
+  </si>
+  <si>
+    <t>public.intro.login.content</t>
+  </si>
+  <si>
+    <t>root.import.upload.error.hint</t>
+  </si>
+  <si>
+    <t>Nahrání importního souboru selhalo. Je možné, že se jedná o dočasnou chybu, zkuste to tedy prosím později.</t>
+  </si>
+  <si>
+    <t>root.import.reset.upload</t>
+  </si>
+  <si>
+    <t>Resetovat</t>
+  </si>
+  <si>
+    <t>public.intro.item.0.title</t>
+  </si>
+  <si>
+    <t>public.intro.item.0.content</t>
+  </si>
+  <si>
+    <t>Pokud chcete aplikaci používat, použijte některou z možností přihlášení. Povolením přístupu aplikace zároveň udělujete souhlas s podmínkami použití.&lt;br/&gt;
+&lt;i&gt;Ve zkratce&lt;/i&gt;: aplikace nevyužívá žádné agresivní způsoby sledování uživatelů.</t>
+  </si>
+  <si>
+    <t>Co nabízí</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Správa buildů&lt;/strong&gt;&lt;br/&gt;
+&lt;i&gt;Build je základní kámen aplikace: díky nim je možné sledovat, co kterému atomizéru sedí a tato možnost otevírá možnosti jednoduchého experimentování a eliminaci případných nepovedených buildů.&lt;/i&gt;&lt;br/&gt;
+&lt;strong&gt;Správa liquidů&lt;/strong&gt;&lt;br/&gt;
+&lt;i&gt;Stejně, jako build, jsou také důležité liquidy: od nástrojů usnadňujících míchání až po trasování zrání a stáří liquidů použitých při vapování může napomoci najít optimální build a správně uzrátý liquid.&lt;/i&gt;&lt;br/&gt;
+&lt;strong&gt;Evidence článků&lt;/strong&gt;&lt;br/&gt;
+&lt;i&gt;Je třeba dbát o svoje zdraví, tudíž aplikace nabízí možnost evidovat články a jejich stáří; vedle evidentního fyzického stavu je možné zapsat data pořízení článků a popsat si je fyzicky.&lt;/i&gt;&lt;br/&gt;
+&lt;strong&gt;Spirálky a odpor&lt;/strong&gt;&lt;br/&gt;
+&lt;i&gt;Aplikace nabízí možnost dopředu odhadnout, jak bude build vypadat a nabídne mnoho dat při plánování buildu. Vše je založeno na vašich datech, tudíž výpočty jsou tak přesné, jak je zadáte.&lt;/i&gt;&lt;br/&gt;
+&lt;strong&gt;Soukromí&lt;/strong&gt;&lt;br/&gt;
+&lt;i&gt;Veškerá data jsou soukromá; neprobíhá žádné sledování ani jiné zneužití dat. Sdílení je možné pouze pokud k němu dáte souhlas.&lt;/i&gt;&lt;br/&gt;</t>
+  </si>
+  <si>
+    <t>public.about.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Tato aplikace vznikla jako praktický pomocník pro všechny kategorie vaperů. Ať už se hodí trasovat buildy a sledovat grafy, nebo třeba jenom evidovat liquidy a jejich složení, nebo jenom stáří atomizérů, vše v této aplikaci naleznete.&lt;/p&gt;
+&lt;p&gt;Za vývojem stojí vapeři, kteří aplikaci prakticky využívají a snaží se ji držet ve formě použitelné co nejsnažším způsobem - veškeré akce kopírují běžnou práci při vapingu, ať už se jedná o míchání liquidů nebo příprava buildů.&lt;/p&gt;
+&lt;p&gt;Jedním ze základních prvků je pak i morální čistota: není přítomné žádné sledování uživatelů, veškerá data jsou ve výchozím stavu privátní.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>public.tos.content</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Použití aplikace&lt;/strong&gt;
+&lt;p&gt;
+V podmínkách není nic složitého: pokud se přihlásíte do aplikace, souhlasíte s použitím základních sušenek (určených pouze pro rozeznání přihlášení) a správou zadaných dat aplikací.
+&lt;/p&gt;
+&lt;p&gt;
+Veškeré zadané údaje do aplikace jsou privátní, nedochází k žádné formě sdílení dat. Systém negeneruje žádná data na pozadí, tzn. vše co systém zná zároveň i vidí jeho uživatel.
+&lt;/p&gt;
+&lt;p&gt;
+Existuje možnost vymazání účtu, která jednoduše odsraní veškerá data spjatá s uživatelem, která je nezvratná.
+&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -5988,10 +6099,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6188,7 +6299,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -6196,7 +6307,7 @@
         <v>1782</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1783</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6204,10 +6315,10 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>1783</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>1784</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>1785</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -6215,10 +6326,10 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>1785</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>1786</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>1787</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -6226,10 +6337,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>1787</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>1788</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>1789</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -6237,10 +6348,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>1789</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>1790</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>1791</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -6248,10 +6359,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>1792</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>1793</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -6259,10 +6370,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -6270,10 +6381,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>1795</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>1796</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>1797</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -6281,10 +6392,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>1798</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>1799</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -6292,10 +6403,76 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>902</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1808</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1809</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1811</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>1202</v>
       </c>
     </row>
   </sheetData>
@@ -6414,10 +6591,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC49E62-0AEE-40E6-B00F-514263105890}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6493,8 +6670,185 @@
         <v>14</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1821</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1823</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1826</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1830</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1842</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1834</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1831</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="230.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="102.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1846</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="166.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1848</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1849</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17366,10 +17720,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17153922-55B5-46AD-9C90-5ED46DB8719C}">
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18204,7 +18558,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
@@ -18215,7 +18569,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
@@ -18226,136 +18580,70 @@
         <v>71</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>1801</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>1802</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>1803</v>
+        <v>1812</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1804</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1805</v>
+        <v>1813</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1806</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>1807</v>
+        <v>1816</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1808</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>1809</v>
+        <v>1837</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1797</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>1810</v>
+        <v>1839</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1811</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>1812</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>1202</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>1814</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>1815</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>1816</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>1817</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>1818</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>1819</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>11</v>
+        <v>1840</v>
       </c>
     </row>
   </sheetData>
@@ -18366,10 +18654,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56FAEBF3-753C-4AE9-A2FF-818B5E33C44A}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19017,6 +19305,17 @@
         <v>42</v>
       </c>
     </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>1815</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Common: Initial boring stuff
</commit_message>
<xml_diff>
--- a/fixtures/translations.xlsx
+++ b/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F92AB72-0A89-4D10-9E17-091D1F5C11DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6CA1F5-3B30-4292-8137-B12DD997DD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="2835" windowWidth="27960" windowHeight="18390" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2070" yWindow="2835" windowWidth="27960" windowHeight="18390" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Translations - Lab" sheetId="7" r:id="rId6"/>
     <sheet name="Translations - Root" sheetId="9" r:id="rId7"/>
     <sheet name="Translations - Shared" sheetId="10" r:id="rId8"/>
+    <sheet name="Translations - Market" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3597" uniqueCount="1850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3641" uniqueCount="1865">
   <si>
     <t>cs</t>
   </si>
@@ -5612,6 +5613,51 @@
 &lt;p&gt;
 Existuje možnost vymazání účtu, která jednoduše odsraní veškerá data spjatá s uživatelem, která je nezvratná.
 &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Translations - Market</t>
+  </si>
+  <si>
+    <t>market.index.title</t>
+  </si>
+  <si>
+    <t>market.home.subtitle</t>
+  </si>
+  <si>
+    <t>Tato část aplikace slouží k získávání předmětů, které již fyzicky vlastníte, ale přejete si je zaevidovat do systému.</t>
+  </si>
+  <si>
+    <t>market.home.menu</t>
+  </si>
+  <si>
+    <t>market.lab.menu</t>
+  </si>
+  <si>
+    <t>market.home.title</t>
+  </si>
+  <si>
+    <t>market.atomizer.menu</t>
+  </si>
+  <si>
+    <t>market.mod.menu</t>
+  </si>
+  <si>
+    <t>market.cotton.menu</t>
+  </si>
+  <si>
+    <t>market.cell.menu</t>
+  </si>
+  <si>
+    <t>market.atomizer.index.title</t>
+  </si>
+  <si>
+    <t>market.mod.index.title</t>
+  </si>
+  <si>
+    <t>market.cotton.index.title</t>
+  </si>
+  <si>
+    <t>market.cell.index.title</t>
   </si>
 </sst>
 </file>
@@ -5965,10 +6011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6120BD2C-6516-4E86-99D3-11A27B514E61}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6038,6 +6084,14 @@
         <v>1773</v>
       </c>
       <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B9" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6593,7 +6647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC49E62-0AEE-40E6-B00F-514263105890}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -18656,8 +18710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56FAEBF3-753C-4AE9-A2FF-818B5E33C44A}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19319,4 +19373,179 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1852</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1854</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1855</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1856</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1857</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1858</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1859</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1860</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1861</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1862</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1864</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Common: Preparing user section under root
</commit_message>
<xml_diff>
--- a/fixtures/translations.xlsx
+++ b/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058A0FD2-EFF5-4CDA-9ABC-D04851DED332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927FD001-E7E6-4F1E-958A-3A9A81CC91FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8115" yWindow="1935" windowWidth="40680" windowHeight="18390" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8115" yWindow="1935" windowWidth="40680" windowHeight="18390" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3659" uniqueCount="1874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3662" uniqueCount="1876">
   <si>
     <t>cs</t>
   </si>
@@ -5686,6 +5686,12 @@
   </si>
   <si>
     <t>market.atomizer.buy.confirm.button</t>
+  </si>
+  <si>
+    <t>root.user.list</t>
+  </si>
+  <si>
+    <t>Seznam uživatelů</t>
   </si>
 </sst>
 </file>
@@ -17813,10 +17819,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17153922-55B5-46AD-9C90-5ED46DB8719C}">
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18737,6 +18743,17 @@
       </c>
       <c r="C83" s="1" t="s">
         <v>1840</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>1874</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>1875</v>
       </c>
     </row>
   </sheetData>
@@ -19418,7 +19435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Common: Improved some things
</commit_message>
<xml_diff>
--- a/fixtures/translations.xlsx
+++ b/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99691292-309E-064E-A179-8B206ECF39AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B5E151-A561-5146-8D85-5045B5CC37E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3683" uniqueCount="1888">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3695" uniqueCount="1896">
   <si>
     <t>cs</t>
   </si>
@@ -5728,6 +5728,30 @@
   </si>
   <si>
     <t>Uživatel</t>
+  </si>
+  <si>
+    <t>root.transaction.amount.label</t>
+  </si>
+  <si>
+    <t>Částka</t>
+  </si>
+  <si>
+    <t>root.transaction.create</t>
+  </si>
+  <si>
+    <t>Vytvořit transakci</t>
+  </si>
+  <si>
+    <t>root.transaction.note.label</t>
+  </si>
+  <si>
+    <t>Poznámka</t>
+  </si>
+  <si>
+    <t>root.transaction.create.success</t>
+  </si>
+  <si>
+    <t>Transakce byla úspěšně vytvořena.</t>
   </si>
 </sst>
 </file>
@@ -17855,10 +17879,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17153922-55B5-46AD-9C90-5ED46DB8719C}">
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18867,6 +18891,50 @@
       </c>
       <c r="C91" s="1" t="s">
         <v>1887</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>1888</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>1890</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>1892</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>1894</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>1895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>